<commit_message>
Added Clear Button and Requirements.txt file
</commit_message>
<xml_diff>
--- a/filtered_data.xlsx
+++ b/filtered_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,16 @@
           <t>Email</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Biometric Verification Completed</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Marksheet X Verification</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -466,6 +476,16 @@
           <t>sanjeev.jadhav99@gmail.com</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -481,6 +501,205 @@
       <c r="C3" t="inlineStr">
         <is>
           <t>rasdas99@gmail.com</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>MBA/0300/61</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SANJIV</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>sanjeev.jadhav99@gmail.com</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>MBA/0300/61</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SANJIV</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>sanjeev.jadhav99@gmail.com</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>MBA/0300/61</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SANJIV</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>sanjeev.jadhav99@gmail.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>MBA/0009/60</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>DHARGAWE SATYATA DILESH</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>satyatad2025@email.iimcal.ac.in</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>MBA/0009/60</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>DHARGAWE SATYATA DILESH</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>satyatad2025@email.iimcal.ac.in</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>MBA/0378/60</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SANJIV AJAY JADHAV</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>sanjivj2025@email.iimcal.ac.in</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>MBA/0378/60</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SANJIV AJAY JADHAV</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>sanjivj2025@email.iimcal.ac.in</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
     </row>

</xml_diff>